<commit_message>
added new features to be used in project reporting
</commit_message>
<xml_diff>
--- a/scr-edu/src/main/resources/poi_templates/export.tmpl.xlsx
+++ b/scr-edu/src/main/resources/poi_templates/export.tmpl.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="28">
   <si>
     <t>Mama plecată</t>
   </si>
@@ -86,6 +86,18 @@
   </si>
   <si>
     <t>Tara unde este plecat parintele</t>
+  </si>
+  <si>
+    <t>Data nașterii</t>
+  </si>
+  <si>
+    <t>Data includerii în proiect</t>
+  </si>
+  <si>
+    <t>Modalitate includere în proiect</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Părinții cu care a comunicat                                          </t>
   </si>
 </sst>
 </file>
@@ -223,23 +235,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -256,11 +275,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -562,438 +577,515 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CK3"/>
+  <dimension ref="A1:CZ3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" customWidth="1"/>
+    <col min="13" max="13" width="9" customWidth="1"/>
+    <col min="14" max="14" width="8" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" customWidth="1"/>
+    <col min="16" max="16" width="8.5703125" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" customWidth="1"/>
+    <col min="19" max="19" width="8.28515625" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" customWidth="1"/>
+    <col min="21" max="21" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="41" width="4.5703125" customWidth="1"/>
-    <col min="42" max="42" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="53" width="4.5703125" customWidth="1"/>
-    <col min="54" max="54" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="5" customWidth="1"/>
-    <col min="56" max="56" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="57" max="65" width="4.5703125" customWidth="1"/>
-    <col min="66" max="66" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="4" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="69" max="77" width="4.5703125" customWidth="1"/>
-    <col min="78" max="78" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="4" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="81" max="89" width="4.5703125" customWidth="1"/>
+    <col min="31" max="32" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="44" width="4.5703125" customWidth="1"/>
+    <col min="45" max="45" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="56" width="4.5703125" customWidth="1"/>
+    <col min="57" max="57" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="5" customWidth="1"/>
+    <col min="59" max="59" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="60" max="68" width="4.5703125" customWidth="1"/>
+    <col min="69" max="69" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="4" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="72" max="80" width="4.5703125" customWidth="1"/>
+    <col min="81" max="81" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="4" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="84" max="92" width="4.5703125" customWidth="1"/>
+    <col min="93" max="93" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="4" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="5" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="103" max="104" width="4.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:104" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="11" t="s">
-        <v>5</v>
-      </c>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
       <c r="AE1" s="11"/>
       <c r="AF1" s="11"/>
-      <c r="AG1" s="11"/>
-      <c r="AH1" s="11"/>
-      <c r="AI1" s="11"/>
-      <c r="AJ1" s="11"/>
-      <c r="AK1" s="11"/>
-      <c r="AL1" s="11"/>
-      <c r="AM1" s="11"/>
-      <c r="AN1" s="11"/>
-      <c r="AO1" s="11"/>
-      <c r="AP1" s="12" t="s">
-        <v>6</v>
-      </c>
+      <c r="AG1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
       <c r="AQ1" s="12"/>
       <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="12"/>
-      <c r="AY1" s="12"/>
-      <c r="AZ1" s="12"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="AS1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AT1" s="13"/>
+      <c r="AU1" s="13"/>
+      <c r="AV1" s="13"/>
+      <c r="AW1" s="13"/>
+      <c r="AX1" s="13"/>
+      <c r="AY1" s="13"/>
+      <c r="AZ1" s="13"/>
+      <c r="BA1" s="13"/>
+      <c r="BB1" s="13"/>
       <c r="BC1" s="13"/>
       <c r="BD1" s="13"/>
-      <c r="BE1" s="13"/>
-      <c r="BF1" s="13"/>
-      <c r="BG1" s="13"/>
-      <c r="BH1" s="13"/>
-      <c r="BI1" s="13"/>
-      <c r="BJ1" s="13"/>
-      <c r="BK1" s="13"/>
-      <c r="BL1" s="13"/>
-      <c r="BM1" s="13"/>
-      <c r="BN1" s="5" t="s">
+      <c r="BE1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="BF1" s="14"/>
+      <c r="BG1" s="14"/>
+      <c r="BH1" s="14"/>
+      <c r="BI1" s="14"/>
+      <c r="BJ1" s="14"/>
+      <c r="BK1" s="14"/>
+      <c r="BL1" s="14"/>
+      <c r="BM1" s="14"/>
+      <c r="BN1" s="14"/>
+      <c r="BO1" s="14"/>
+      <c r="BP1" s="14"/>
+      <c r="BQ1" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="BR1" s="15"/>
+      <c r="BS1" s="15"/>
+      <c r="BT1" s="15"/>
+      <c r="BU1" s="15"/>
+      <c r="BV1" s="15"/>
+      <c r="BW1" s="15"/>
+      <c r="BX1" s="15"/>
+      <c r="BY1" s="15"/>
+      <c r="BZ1" s="15"/>
+      <c r="CA1" s="15"/>
+      <c r="CB1" s="15"/>
+      <c r="CC1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="BO1" s="5"/>
-      <c r="BP1" s="5"/>
-      <c r="BQ1" s="5"/>
-      <c r="BR1" s="5"/>
-      <c r="BS1" s="5"/>
-      <c r="BT1" s="5"/>
-      <c r="BU1" s="5"/>
-      <c r="BV1" s="5"/>
-      <c r="BW1" s="5"/>
-      <c r="BX1" s="5"/>
-      <c r="BY1" s="5"/>
-      <c r="BZ1" s="6" t="s">
+      <c r="CD1" s="9"/>
+      <c r="CE1" s="9"/>
+      <c r="CF1" s="9"/>
+      <c r="CG1" s="9"/>
+      <c r="CH1" s="9"/>
+      <c r="CI1" s="9"/>
+      <c r="CJ1" s="9"/>
+      <c r="CK1" s="9"/>
+      <c r="CL1" s="9"/>
+      <c r="CM1" s="9"/>
+      <c r="CN1" s="9"/>
+      <c r="CO1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="CA1" s="6"/>
-      <c r="CB1" s="6"/>
-      <c r="CC1" s="6"/>
-      <c r="CD1" s="6"/>
-      <c r="CE1" s="6"/>
-      <c r="CF1" s="6"/>
-      <c r="CG1" s="6"/>
-      <c r="CH1" s="6"/>
-      <c r="CI1" s="6"/>
-      <c r="CJ1" s="6"/>
-      <c r="CK1" s="6"/>
+      <c r="CP1" s="10"/>
+      <c r="CQ1" s="10"/>
+      <c r="CR1" s="10"/>
+      <c r="CS1" s="10"/>
+      <c r="CT1" s="10"/>
+      <c r="CU1" s="10"/>
+      <c r="CV1" s="10"/>
+      <c r="CW1" s="10"/>
+      <c r="CX1" s="10"/>
+      <c r="CY1" s="10"/>
+      <c r="CZ1" s="10"/>
     </row>
-    <row r="2" spans="1:89" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="8"/>
+    <row r="2" spans="1:104" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
       <c r="E2" s="8"/>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AL2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AM2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AN2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AO2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AP2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AR2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AT2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AU2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AV2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AW2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AX2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AV2" s="3" t="s">
+      <c r="AY2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AW2" s="3" t="s">
+      <c r="AZ2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AX2" s="3" t="s">
+      <c r="BA2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AY2" s="3" t="s">
+      <c r="BB2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AZ2" s="3" t="s">
+      <c r="BC2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="BA2" s="3" t="s">
+      <c r="BD2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="BB2" s="2" t="s">
+      <c r="BE2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="BC2" s="3" t="s">
+      <c r="BF2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="BD2" s="3" t="s">
+      <c r="BG2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="BE2" s="3" t="s">
+      <c r="BH2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="BF2" s="3" t="s">
+      <c r="BI2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="BG2" s="3" t="s">
+      <c r="BJ2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="BH2" s="3" t="s">
+      <c r="BK2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="BI2" s="3" t="s">
+      <c r="BL2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="BJ2" s="3" t="s">
+      <c r="BM2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="BK2" s="3" t="s">
+      <c r="BN2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="BL2" s="3" t="s">
+      <c r="BO2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="BM2" s="3" t="s">
+      <c r="BP2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="BN2" s="2" t="s">
+      <c r="BQ2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="BO2" s="3" t="s">
+      <c r="BR2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="BP2" s="3" t="s">
+      <c r="BS2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="BQ2" s="3" t="s">
+      <c r="BT2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="BR2" s="3" t="s">
+      <c r="BU2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="BS2" s="3" t="s">
+      <c r="BV2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="BT2" s="3" t="s">
+      <c r="BW2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="BU2" s="3" t="s">
+      <c r="BX2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="BV2" s="3" t="s">
+      <c r="BY2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="BW2" s="3" t="s">
+      <c r="BZ2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="BX2" s="3" t="s">
+      <c r="CA2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="BY2" s="3" t="s">
+      <c r="CB2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="BZ2" s="2" t="s">
+      <c r="CC2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="CA2" s="3" t="s">
+      <c r="CD2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="CB2" s="3" t="s">
+      <c r="CE2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="CC2" s="3" t="s">
+      <c r="CF2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="CD2" s="3" t="s">
+      <c r="CG2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="CE2" s="3" t="s">
+      <c r="CH2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="CF2" s="3" t="s">
+      <c r="CI2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="CG2" s="3" t="s">
+      <c r="CJ2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="CH2" s="3" t="s">
+      <c r="CK2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="CI2" s="3" t="s">
+      <c r="CL2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="CJ2" s="3" t="s">
+      <c r="CM2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="CK2" s="3" t="s">
+      <c r="CN2" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="CO2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="CP2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="CQ2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="CR2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="CS2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="CT2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="CU2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="CV2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="CW2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="CX2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="CY2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="CZ2" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:89" ht="30" customHeight="1">
+    <row r="3" spans="1:104" ht="30" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1083,21 +1175,40 @@
       <c r="CI3" s="4"/>
       <c r="CJ3" s="4"/>
       <c r="CK3" s="4"/>
+      <c r="CL3" s="4"/>
+      <c r="CM3" s="4"/>
+      <c r="CN3" s="4"/>
+      <c r="CO3" s="4"/>
+      <c r="CP3" s="4"/>
+      <c r="CQ3" s="4"/>
+      <c r="CR3" s="4"/>
+      <c r="CS3" s="4"/>
+      <c r="CT3" s="4"/>
+      <c r="CU3" s="4"/>
+      <c r="CV3" s="4"/>
+      <c r="CW3" s="4"/>
+      <c r="CX3" s="4"/>
+      <c r="CY3" s="4"/>
+      <c r="CZ3" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="CO1:CZ1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="U1:AF1"/>
+    <mergeCell ref="AG1:AR1"/>
+    <mergeCell ref="AS1:BD1"/>
+    <mergeCell ref="BE1:BP1"/>
+    <mergeCell ref="BQ1:CB1"/>
+    <mergeCell ref="I1:T1"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="BN1:BY1"/>
-    <mergeCell ref="BZ1:CK1"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:Q1"/>
-    <mergeCell ref="R1:AC1"/>
-    <mergeCell ref="AD1:AO1"/>
-    <mergeCell ref="AP1:BA1"/>
-    <mergeCell ref="BB1:BM1"/>
+    <mergeCell ref="CC1:CN1"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added inaictivity checkboxes, nrcrt columns and date validation + update reports and exports. disabled import
</commit_message>
<xml_diff>
--- a/scr-edu/src/main/resources/poi_templates/export.tmpl.xlsx
+++ b/scr-edu/src/main/resources/poi_templates/export.tmpl.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="31">
   <si>
     <t>Mama plecată</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Părinții cu care a comunicat                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Minim o activitate                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Inactiv                                      </t>
+  </si>
+  <si>
+    <t>Nr.Crt.</t>
   </si>
 </sst>
 </file>
@@ -241,24 +250,14 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -277,6 +276,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,515 +586,649 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CZ3"/>
+  <dimension ref="A1:DY3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" customWidth="1"/>
-    <col min="13" max="13" width="9" customWidth="1"/>
-    <col min="14" max="14" width="8" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" customWidth="1"/>
-    <col min="16" max="16" width="8.5703125" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" customWidth="1"/>
-    <col min="19" max="19" width="8.28515625" customWidth="1"/>
-    <col min="20" max="20" width="9.5703125" customWidth="1"/>
-    <col min="21" max="21" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="44" width="4.5703125" customWidth="1"/>
-    <col min="45" max="45" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="48" max="56" width="4.5703125" customWidth="1"/>
-    <col min="57" max="57" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="5" customWidth="1"/>
-    <col min="59" max="59" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="60" max="68" width="4.5703125" customWidth="1"/>
-    <col min="69" max="69" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="4" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="72" max="80" width="4.5703125" customWidth="1"/>
-    <col min="81" max="81" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="4" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="84" max="92" width="4.5703125" customWidth="1"/>
-    <col min="93" max="93" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="4" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="5" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="103" max="104" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" customWidth="1"/>
+    <col min="13" max="13" width="6.5703125" customWidth="1"/>
+    <col min="14" max="14" width="7" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" customWidth="1"/>
+    <col min="16" max="16" width="6.5703125" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="18" width="7.140625" customWidth="1"/>
+    <col min="19" max="19" width="6.140625" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" customWidth="1"/>
+    <col min="22" max="22" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="57" width="4.5703125" customWidth="1"/>
+    <col min="58" max="58" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="5" customWidth="1"/>
+    <col min="60" max="60" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="61" max="69" width="4.5703125" customWidth="1"/>
+    <col min="70" max="70" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="4" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="81" width="4.5703125" customWidth="1"/>
+    <col min="82" max="82" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="4" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="85" max="93" width="4.5703125" customWidth="1"/>
+    <col min="94" max="94" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="4" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="5" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="104" max="105" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="4" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="5" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="116" max="117" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="4" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="5" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="128" max="129" width="4.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:104" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:129" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A1" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="11" t="s">
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI1" s="13"/>
+      <c r="AJ1" s="13"/>
+      <c r="AK1" s="13"/>
+      <c r="AL1" s="13"/>
+      <c r="AM1" s="13"/>
+      <c r="AN1" s="13"/>
+      <c r="AO1" s="13"/>
+      <c r="AP1" s="13"/>
+      <c r="AQ1" s="13"/>
+      <c r="AR1" s="13"/>
+      <c r="AS1" s="13"/>
+      <c r="AT1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11"/>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="11"/>
-      <c r="AG1" s="12" t="s">
+      <c r="AU1" s="8"/>
+      <c r="AV1" s="8"/>
+      <c r="AW1" s="8"/>
+      <c r="AX1" s="8"/>
+      <c r="AY1" s="8"/>
+      <c r="AZ1" s="8"/>
+      <c r="BA1" s="8"/>
+      <c r="BB1" s="8"/>
+      <c r="BC1" s="8"/>
+      <c r="BD1" s="8"/>
+      <c r="BE1" s="8"/>
+      <c r="BF1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="13" t="s">
+      <c r="BG1" s="9"/>
+      <c r="BH1" s="9"/>
+      <c r="BI1" s="9"/>
+      <c r="BJ1" s="9"/>
+      <c r="BK1" s="9"/>
+      <c r="BL1" s="9"/>
+      <c r="BM1" s="9"/>
+      <c r="BN1" s="9"/>
+      <c r="BO1" s="9"/>
+      <c r="BP1" s="9"/>
+      <c r="BQ1" s="9"/>
+      <c r="BR1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="AT1" s="13"/>
-      <c r="AU1" s="13"/>
-      <c r="AV1" s="13"/>
-      <c r="AW1" s="13"/>
-      <c r="AX1" s="13"/>
-      <c r="AY1" s="13"/>
-      <c r="AZ1" s="13"/>
-      <c r="BA1" s="13"/>
-      <c r="BB1" s="13"/>
-      <c r="BC1" s="13"/>
-      <c r="BD1" s="13"/>
-      <c r="BE1" s="14" t="s">
+      <c r="BS1" s="10"/>
+      <c r="BT1" s="10"/>
+      <c r="BU1" s="10"/>
+      <c r="BV1" s="10"/>
+      <c r="BW1" s="10"/>
+      <c r="BX1" s="10"/>
+      <c r="BY1" s="10"/>
+      <c r="BZ1" s="10"/>
+      <c r="CA1" s="10"/>
+      <c r="CB1" s="10"/>
+      <c r="CC1" s="10"/>
+      <c r="CD1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="BF1" s="14"/>
-      <c r="BG1" s="14"/>
-      <c r="BH1" s="14"/>
-      <c r="BI1" s="14"/>
-      <c r="BJ1" s="14"/>
-      <c r="BK1" s="14"/>
-      <c r="BL1" s="14"/>
-      <c r="BM1" s="14"/>
-      <c r="BN1" s="14"/>
-      <c r="BO1" s="14"/>
-      <c r="BP1" s="14"/>
-      <c r="BQ1" s="15" t="s">
+      <c r="CE1" s="11"/>
+      <c r="CF1" s="11"/>
+      <c r="CG1" s="11"/>
+      <c r="CH1" s="11"/>
+      <c r="CI1" s="11"/>
+      <c r="CJ1" s="11"/>
+      <c r="CK1" s="11"/>
+      <c r="CL1" s="11"/>
+      <c r="CM1" s="11"/>
+      <c r="CN1" s="11"/>
+      <c r="CO1" s="11"/>
+      <c r="CP1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="BR1" s="15"/>
-      <c r="BS1" s="15"/>
-      <c r="BT1" s="15"/>
-      <c r="BU1" s="15"/>
-      <c r="BV1" s="15"/>
-      <c r="BW1" s="15"/>
-      <c r="BX1" s="15"/>
-      <c r="BY1" s="15"/>
-      <c r="BZ1" s="15"/>
-      <c r="CA1" s="15"/>
-      <c r="CB1" s="15"/>
-      <c r="CC1" s="9" t="s">
+      <c r="CQ1" s="12"/>
+      <c r="CR1" s="12"/>
+      <c r="CS1" s="12"/>
+      <c r="CT1" s="12"/>
+      <c r="CU1" s="12"/>
+      <c r="CV1" s="12"/>
+      <c r="CW1" s="12"/>
+      <c r="CX1" s="12"/>
+      <c r="CY1" s="12"/>
+      <c r="CZ1" s="12"/>
+      <c r="DA1" s="12"/>
+      <c r="DB1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="CD1" s="9"/>
-      <c r="CE1" s="9"/>
-      <c r="CF1" s="9"/>
-      <c r="CG1" s="9"/>
-      <c r="CH1" s="9"/>
-      <c r="CI1" s="9"/>
-      <c r="CJ1" s="9"/>
-      <c r="CK1" s="9"/>
-      <c r="CL1" s="9"/>
-      <c r="CM1" s="9"/>
-      <c r="CN1" s="9"/>
-      <c r="CO1" s="10" t="s">
+      <c r="DC1" s="16"/>
+      <c r="DD1" s="16"/>
+      <c r="DE1" s="16"/>
+      <c r="DF1" s="16"/>
+      <c r="DG1" s="16"/>
+      <c r="DH1" s="16"/>
+      <c r="DI1" s="16"/>
+      <c r="DJ1" s="16"/>
+      <c r="DK1" s="16"/>
+      <c r="DL1" s="16"/>
+      <c r="DM1" s="16"/>
+      <c r="DN1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="CP1" s="10"/>
-      <c r="CQ1" s="10"/>
-      <c r="CR1" s="10"/>
-      <c r="CS1" s="10"/>
-      <c r="CT1" s="10"/>
-      <c r="CU1" s="10"/>
-      <c r="CV1" s="10"/>
-      <c r="CW1" s="10"/>
-      <c r="CX1" s="10"/>
-      <c r="CY1" s="10"/>
-      <c r="CZ1" s="10"/>
+      <c r="DO1" s="5"/>
+      <c r="DP1" s="5"/>
+      <c r="DQ1" s="5"/>
+      <c r="DR1" s="5"/>
+      <c r="DS1" s="5"/>
+      <c r="DT1" s="5"/>
+      <c r="DU1" s="5"/>
+      <c r="DV1" s="5"/>
+      <c r="DW1" s="5"/>
+      <c r="DX1" s="5"/>
+      <c r="DY1" s="5"/>
     </row>
-    <row r="2" spans="1:104" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="2" t="s">
+    <row r="2" spans="1:129" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AG2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AL2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AM2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AN2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AO2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AP2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AR2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AS2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AS2" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AU2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AV2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AV2" s="3" t="s">
+      <c r="AW2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AW2" s="3" t="s">
+      <c r="AX2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AX2" s="3" t="s">
+      <c r="AY2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AY2" s="3" t="s">
+      <c r="AZ2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AZ2" s="3" t="s">
+      <c r="BA2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="BA2" s="3" t="s">
+      <c r="BB2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="BB2" s="3" t="s">
+      <c r="BC2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="BC2" s="3" t="s">
+      <c r="BD2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="BD2" s="3" t="s">
+      <c r="BE2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="BE2" s="2" t="s">
+      <c r="BF2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="BF2" s="3" t="s">
+      <c r="BG2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="BG2" s="3" t="s">
+      <c r="BH2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="BH2" s="3" t="s">
+      <c r="BI2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="BI2" s="3" t="s">
+      <c r="BJ2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="BJ2" s="3" t="s">
+      <c r="BK2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="BK2" s="3" t="s">
+      <c r="BL2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="BL2" s="3" t="s">
+      <c r="BM2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="BM2" s="3" t="s">
+      <c r="BN2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="BN2" s="3" t="s">
+      <c r="BO2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="BO2" s="3" t="s">
+      <c r="BP2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="BP2" s="3" t="s">
+      <c r="BQ2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="BQ2" s="2" t="s">
+      <c r="BR2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="BR2" s="3" t="s">
+      <c r="BS2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="BS2" s="3" t="s">
+      <c r="BT2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="BT2" s="3" t="s">
+      <c r="BU2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="BU2" s="3" t="s">
+      <c r="BV2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="BV2" s="3" t="s">
+      <c r="BW2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="BW2" s="3" t="s">
+      <c r="BX2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="BX2" s="3" t="s">
+      <c r="BY2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="BY2" s="3" t="s">
+      <c r="BZ2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="BZ2" s="3" t="s">
+      <c r="CA2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="CA2" s="3" t="s">
+      <c r="CB2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="CB2" s="3" t="s">
+      <c r="CC2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="CC2" s="2" t="s">
+      <c r="CD2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="CD2" s="3" t="s">
+      <c r="CE2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="CE2" s="3" t="s">
+      <c r="CF2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="CF2" s="3" t="s">
+      <c r="CG2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="CG2" s="3" t="s">
+      <c r="CH2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="CH2" s="3" t="s">
+      <c r="CI2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="CI2" s="3" t="s">
+      <c r="CJ2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="CJ2" s="3" t="s">
+      <c r="CK2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="CK2" s="3" t="s">
+      <c r="CL2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="CL2" s="3" t="s">
+      <c r="CM2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="CM2" s="3" t="s">
+      <c r="CN2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="CN2" s="3" t="s">
+      <c r="CO2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="CO2" s="2" t="s">
+      <c r="CP2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="CP2" s="3" t="s">
+      <c r="CQ2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="CQ2" s="3" t="s">
+      <c r="CR2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="CR2" s="3" t="s">
+      <c r="CS2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="CS2" s="3" t="s">
+      <c r="CT2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="CT2" s="3" t="s">
+      <c r="CU2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="CU2" s="3" t="s">
+      <c r="CV2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="CV2" s="3" t="s">
+      <c r="CW2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="CW2" s="3" t="s">
+      <c r="CX2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="CX2" s="3" t="s">
+      <c r="CY2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="CY2" s="3" t="s">
+      <c r="CZ2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="CZ2" s="3" t="s">
+      <c r="DA2" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="DB2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="DC2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="DD2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="DE2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="DF2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="DG2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="DH2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="DI2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="DJ2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="DK2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="DL2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="DM2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="DN2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="DO2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="DP2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="DQ2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="DR2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="DS2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="DT2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="DU2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="DV2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="DW2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="DX2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="DY2" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:104" ht="30" customHeight="1">
+    <row r="3" spans="1:129" ht="30" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1190,25 +1333,53 @@
       <c r="CX3" s="4"/>
       <c r="CY3" s="4"/>
       <c r="CZ3" s="4"/>
+      <c r="DA3" s="4"/>
+      <c r="DB3" s="4"/>
+      <c r="DC3" s="4"/>
+      <c r="DD3" s="4"/>
+      <c r="DE3" s="4"/>
+      <c r="DF3" s="4"/>
+      <c r="DG3" s="4"/>
+      <c r="DH3" s="4"/>
+      <c r="DI3" s="4"/>
+      <c r="DJ3" s="4"/>
+      <c r="DK3" s="4"/>
+      <c r="DL3" s="4"/>
+      <c r="DM3" s="4"/>
+      <c r="DN3" s="4"/>
+      <c r="DO3" s="4"/>
+      <c r="DP3" s="4"/>
+      <c r="DQ3" s="4"/>
+      <c r="DR3" s="4"/>
+      <c r="DS3" s="4"/>
+      <c r="DT3" s="4"/>
+      <c r="DU3" s="4"/>
+      <c r="DV3" s="4"/>
+      <c r="DW3" s="4"/>
+      <c r="DX3" s="4"/>
+      <c r="DY3" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="CO1:CZ1"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="U1:AF1"/>
-    <mergeCell ref="AG1:AR1"/>
-    <mergeCell ref="AS1:BD1"/>
-    <mergeCell ref="BE1:BP1"/>
-    <mergeCell ref="BQ1:CB1"/>
-    <mergeCell ref="I1:T1"/>
+  <mergeCells count="19">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="CC1:CN1"/>
-    <mergeCell ref="B1:B2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="DB1:DM1"/>
+    <mergeCell ref="C1:C2"/>
     <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="J1:U1"/>
+    <mergeCell ref="V1:AG1"/>
+    <mergeCell ref="DN1:DY1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="AT1:BE1"/>
+    <mergeCell ref="BF1:BQ1"/>
+    <mergeCell ref="BR1:CC1"/>
+    <mergeCell ref="CD1:CO1"/>
+    <mergeCell ref="CP1:DA1"/>
+    <mergeCell ref="AH1:AS1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>